<commit_message>
check combine_with_other_tools - parse
</commit_message>
<xml_diff>
--- a/data/procon/combine_with_other_tools - parse - variant.xlsx
+++ b/data/procon/combine_with_other_tools - parse - variant.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box\Cov2_protein\data\procon\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCB69E7-01CD-4ED7-89EB-031315225E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -115,12 +121,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,8 +134,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -168,22 +181,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -225,7 +249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,9 +281,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,6 +333,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,14 +526,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -493,14 +563,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -510,13 +580,13 @@
         <v>-0.8999999999999998</v>
       </c>
       <c r="F2">
-        <v>0.0373860734684987</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+        <v>3.7386073468498697E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
@@ -524,14 +594,14 @@
         <v>0.8999999999999998</v>
       </c>
       <c r="F3">
-        <v>0.0373860734684987</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+        <v>3.7386073468498697E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -541,15 +611,15 @@
         <v>28</v>
       </c>
       <c r="E4">
-        <v>0.7714285714285712</v>
+        <v>0.77142857142857124</v>
       </c>
       <c r="F4">
-        <v>0.0007568751073803</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+        <v>7.5687510738030003E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
@@ -557,13 +627,13 @@
         <v>29</v>
       </c>
       <c r="E5">
-        <v>0.6666666666666667</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="F5">
-        <v>0.0498672305688851</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>4.9867230568885097E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -577,81 +647,81 @@
         <v>30</v>
       </c>
       <c r="E6">
-        <v>0.7857142857142859</v>
+        <v>0.78571428571428592</v>
       </c>
       <c r="F6">
-        <v>0.0362384626798271</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
+        <v>3.6238462679827103E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E7">
-        <v>0.8571428571428573</v>
+        <v>0.85714285714285732</v>
       </c>
       <c r="F7">
-        <v>0.0136973266153256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+        <v>1.36973266153256E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E8">
-        <v>0.7857142857142859</v>
+        <v>0.78571428571428592</v>
       </c>
       <c r="F8">
-        <v>0.0362384626798271</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
+        <v>3.6238462679827103E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E9">
-        <v>0.7857142857142858</v>
+        <v>0.78571428571428581</v>
       </c>
       <c r="F9">
-        <v>0.0208151272535252</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>2.08151272535252E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E10">
-        <v>0.7142857142857144</v>
+        <v>0.71428571428571441</v>
       </c>
       <c r="F10">
-        <v>0.0465282322841672</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>4.6528232284167199E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -665,48 +735,48 @@
         <v>28</v>
       </c>
       <c r="E11">
-        <v>0.7818181818181817</v>
+        <v>0.78181818181818175</v>
       </c>
       <c r="F11">
-        <v>0.0075470077810678</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
+        <v>7.5470077810678004E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E12">
-        <v>0.4058119658119658</v>
+        <v>0.40581196581196582</v>
       </c>
       <c r="F12">
-        <v>0.0396921214910413</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+        <v>3.9692121491041302E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E13">
-        <v>-0.4058119658119658</v>
+        <v>-0.40581196581196582</v>
       </c>
       <c r="F13">
-        <v>0.0396921214910413</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
+        <v>3.9692121491041302E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -719,14 +789,14 @@
         <v>28</v>
       </c>
       <c r="E14">
-        <v>0.2192244020992568</v>
+        <v>0.21922440209925681</v>
       </c>
       <c r="F14">
-        <v>0.0401563006124572</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1"/>
+        <v>4.0156300612457202E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -737,14 +807,14 @@
         <v>29</v>
       </c>
       <c r="E15">
-        <v>0.4236453201970443</v>
+        <v>0.42364532019704432</v>
       </c>
       <c r="F15">
-        <v>0.0246716626723123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
+        <v>2.46716626723123E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -760,11 +830,11 @@
         <v>0.2214182820924393</v>
       </c>
       <c r="F16">
-        <v>0.035966739962233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1"/>
+        <v>3.5966739962232999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
@@ -778,16 +848,15 @@
         <v>0.4458128078817733</v>
       </c>
       <c r="F17">
-        <v>0.0153574942919786</v>
+        <v>1.53574942919786E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B2:B3"/>
@@ -795,11 +864,13 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change shortest path length; and update reuslt;
</commit_message>
<xml_diff>
--- a/data/procon/combine_with_other_tools - parse - variant.xlsx
+++ b/data/procon/combine_with_other_tools - parse - variant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box\Cov2_protein\data\procon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCB69E7-01CD-4ED7-89EB-031315225E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B8F1E8-D036-4427-A705-B88976CC50BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
   <si>
     <t>Correlation</t>
   </si>
@@ -46,16 +46,28 @@
     <t>AV.1</t>
   </si>
   <si>
+    <t>AY.4.2</t>
+  </si>
+  <si>
+    <t>B.1.1.318</t>
+  </si>
+  <si>
     <t>B.1.1.7+L452R</t>
   </si>
   <si>
     <t>B.1.351(Beta)</t>
   </si>
   <si>
+    <t>B.1.351+E516Q</t>
+  </si>
+  <si>
     <t>B.1.351+P384L</t>
   </si>
   <si>
-    <t>B.1.621(Mu)</t>
+    <t>B.1.617.2(Delta)</t>
+  </si>
+  <si>
+    <t>B.1.617.3</t>
   </si>
   <si>
     <t>BA.1(Omicron)</t>
@@ -67,6 +79,9 @@
     <t>BA.4(Omicron)</t>
   </si>
   <si>
+    <t>P.1(Gamma)</t>
+  </si>
+  <si>
     <t>BFE</t>
   </si>
   <si>
@@ -76,37 +91,55 @@
     <t>V367F(8.02),F157L(7.76),Q613H(7.09)</t>
   </si>
   <si>
-    <t>T95I-G142D(-2.98),T95I-N439K(-1.58),D80G-T95I(-1.38)</t>
+    <t>F157L-V367F(7.89),V367F-Q613H(7.55),V367F-E484K(7.46)</t>
   </si>
   <si>
     <t>G142D(-4.78),N439K(-1.98),D80G(-1.58)</t>
   </si>
   <si>
+    <t>D80G-D614G(7.87),N439K-D614G(7.50),D614G-E484K(7.45)</t>
+  </si>
+  <si>
+    <t>T478K-D614G(8.02),E156G-T478K(7.72),E156G-D614G(7.70)</t>
+  </si>
+  <si>
+    <t>D614G-D796H(7.49),D614G-E484K(7.45),T95I-D614G(7.30)</t>
+  </si>
+  <si>
     <t>D614G(8.00),S982A(7.52),T716I(6.54)</t>
   </si>
   <si>
     <t>D215G(8.10),D614G(8.00),D80A(7.74)</t>
   </si>
   <si>
-    <t>R346K-D614G(7.56),T95I-D614G(7.30),Y145N-D614G(7.10)</t>
+    <t>D215G-D614G(8.05),D80A-D215G(7.92),D215G-A701V(7.92)</t>
+  </si>
+  <si>
+    <t>T19R-L452R(-1.01),T19R-E484Q(-0.90),L452R-E484Q(-0.82)</t>
+  </si>
+  <si>
+    <t>Q493R-T547K(8.15),T478K-Q493R(8.13),Q493R-D614G(8.12)</t>
   </si>
   <si>
     <t>Q493R(8.23),T547K(8.07),T478K(8.04)</t>
   </si>
   <si>
-    <t>S371F-D614G(7.99),S375F-D614G(7.97),S477N-T478K(7.97)</t>
+    <t>T478K-Q493R(8.13),V213G-Q493R(8.12),Q493R-D614G(8.12)</t>
   </si>
   <si>
     <t>G142D(-4.78),V213G(-1.79),T376A(-1.67)</t>
   </si>
   <si>
-    <t>average shortest length</t>
+    <t>V213G-T478K(8.02),T478K-D614G(8.02),S371F-T478K(8.01)</t>
+  </si>
+  <si>
+    <t>L18F-R190S(-1.50),R190S-E484K(-1.39),R190S-N501Y(-1.38)</t>
   </si>
   <si>
     <t>closeness centrality</t>
   </si>
   <si>
-    <t>co-conservation</t>
+    <t>shortest path length</t>
   </si>
   <si>
     <t>page rank</t>
@@ -122,6 +155,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -181,11 +217,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -527,18 +564,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
@@ -564,73 +601,77 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2">
-        <v>-0.8999999999999998</v>
-      </c>
-      <c r="F2">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.8999999999999998</v>
+      </c>
+      <c r="F2" s="2">
         <v>3.7386073468498697E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3">
-        <v>0.8999999999999998</v>
-      </c>
-      <c r="F3">
-        <v>3.7386073468498697E-2</v>
+        <v>39</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-0.79393939393939383</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6.0999233136969002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4">
-        <v>0.77142857142857124</v>
-      </c>
-      <c r="F4">
-        <v>7.5687510738030003E-4</v>
+        <v>40</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4.9867230568885097E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5">
-        <v>0.66666666666666674</v>
-      </c>
-      <c r="F5">
-        <v>4.9867230568885097E-2</v>
+        <v>39</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-0.5025974025974026</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.02298287710122E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -638,239 +679,356 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.3880952380952381</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3.4138671646871E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-0.66060606060606053</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3.7588377571409301E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.78571428571428592</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.6238462679827103E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.78571428571428592</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3.6238462679827103E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-0.59740259740259738</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4.2408741172226998E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.85714285714285732</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.36973266153256E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-0.38642583470169672</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4.2232324698401401E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.78571428571428581</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2.08151272535252E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.71428571428571441</v>
+      </c>
+      <c r="F14" s="2">
+        <v>4.6528232284167199E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.45584415584415577</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3.7819989003877501E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6">
-        <v>0.78571428571428592</v>
-      </c>
-      <c r="F6">
-        <v>3.6238462679827103E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7">
-        <v>0.85714285714285732</v>
-      </c>
-      <c r="F7">
-        <v>1.36973266153256E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8">
-        <v>0.78571428571428592</v>
-      </c>
-      <c r="F8">
-        <v>3.6238462679827103E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.70909090909090899</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2.16659233675324E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.27457031396451209</v>
+      </c>
+      <c r="F17" s="2">
+        <v>4.9621257569680116E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-0.40581196581196582</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3.9692121491041302E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.30363941613941609</v>
+      </c>
+      <c r="F19" s="2">
+        <v>6.3969284446421424E-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9">
-        <v>0.78571428571428581</v>
-      </c>
-      <c r="F9">
-        <v>2.08151272535252E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10">
-        <v>0.71428571428571441</v>
-      </c>
-      <c r="F10">
-        <v>4.6528232284167199E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11">
-        <v>0.78181818181818175</v>
-      </c>
-      <c r="F11">
-        <v>7.5470077810678004E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12">
-        <v>0.40581196581196582</v>
-      </c>
-      <c r="F12">
-        <v>3.9692121491041302E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13">
-        <v>-0.40581196581196582</v>
-      </c>
-      <c r="F13">
-        <v>3.9692121491041302E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14">
-        <v>0.21922440209925681</v>
-      </c>
-      <c r="F14">
-        <v>4.0156300612457202E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15">
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="2">
         <v>0.42364532019704432</v>
       </c>
-      <c r="F15">
+      <c r="F20" s="2">
         <v>2.46716626723123E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16">
-        <v>0.2214182820924393</v>
-      </c>
-      <c r="F16">
-        <v>3.5966739962232999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.22326293514556869</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.177117838981658E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="2">
         <v>0.4458128078817733</v>
       </c>
-      <c r="F17">
+      <c r="F22" s="2">
         <v>1.53574942919786E-2</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="2">
+        <v>-0.42194365876068018</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4.176009039915E-4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
+  <mergeCells count="12">
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>